<commit_message>
1º funcionalidade em processo
</commit_message>
<xml_diff>
--- a/Scrum/Work breakdown structure.xlsx
+++ b/Scrum/Work breakdown structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\ES\ES_gantProject\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2F2CB6-C027-427E-B0AE-94BC5F0CB9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8256D7FC-93CF-4FC6-9180-343CC82A2510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Task ID</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>60152 code smells</t>
+  </si>
+  <si>
+    <t>1º functionality</t>
+  </si>
+  <si>
+    <t>2º functionality</t>
+  </si>
+  <si>
+    <t>use cases</t>
+  </si>
+  <si>
+    <t>demo video</t>
+  </si>
+  <si>
+    <t>final delivarable</t>
   </si>
 </sst>
 </file>
@@ -104,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -119,21 +134,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -258,36 +258,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -570,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C14"/>
+  <dimension ref="B2:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,16 +580,16 @@
   <sheetData>
     <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -666,12 +663,52 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
+    <row r="14" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>